<commit_message>
Finished adding filtering to tables. Preparing for polymer integration on filtering
</commit_message>
<xml_diff>
--- a/UCosmic.Web.Mvc/App_Data/uploads/testdata.xlsx
+++ b/UCosmic.Web.Mvc/App_Data/uploads/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4020"/>
   </bookViews>
   <sheets>
     <sheet name="StudentActivity" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="36">
   <si>
     <t>externalId</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Computer Engineering</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
     <t>OUT</t>
   </si>
   <si>
@@ -90,6 +87,51 @@
   </si>
   <si>
     <t>Fall 2014</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>University of South Florida</t>
+  </si>
+  <si>
+    <t>Beijing University of Technology</t>
+  </si>
+  <si>
+    <t>Sun Yat-Sen University</t>
+  </si>
+  <si>
+    <t>Spring 2013</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>State University of New York (SUNY)</t>
+  </si>
+  <si>
+    <t>EG</t>
+  </si>
+  <si>
+    <t>Future University in Egypt</t>
+  </si>
+  <si>
+    <t>Political Science</t>
+  </si>
+  <si>
+    <t>Spring 2012</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>Economics :)</t>
+  </si>
+  <si>
+    <t>Finance :D</t>
+  </si>
+  <si>
+    <t>Civil Engineering</t>
   </si>
 </sst>
 </file>
@@ -408,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,18 +461,19 @@
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,37 +484,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>109136</v>
       </c>
@@ -481,76 +527,566 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
         <v>41985</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>41876</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>14.0801</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
       </c>
       <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2">
+        <v>179</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>109137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1">
+        <v>42350</v>
+      </c>
+      <c r="G3" s="1">
+        <v>42241</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
         <v>14.0801</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>109136</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1">
-        <v>42350</v>
-      </c>
-      <c r="F3" s="1">
-        <v>42241</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3">
-        <v>14.0801</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="K3">
-        <v>14.0801</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3">
+        <v>179</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>109138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1">
+        <v>41395</v>
+      </c>
+      <c r="G4" s="1">
+        <v>41275</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4">
+        <v>12.0123</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1298</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1">
+        <v>40909</v>
+      </c>
+      <c r="G5" s="1">
+        <v>41030</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5">
+        <v>12.0121</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5">
+        <v>161</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1">
+        <v>41395</v>
+      </c>
+      <c r="G6" s="1">
+        <v>41275</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6">
+        <v>12.0123</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1">
+        <v>40909</v>
+      </c>
+      <c r="G7" s="1">
+        <v>41030</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7">
+        <v>12.0121</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7">
+        <v>161</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1">
+        <v>40909</v>
+      </c>
+      <c r="G8" s="1">
+        <v>41030</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8">
+        <v>12.0121</v>
+      </c>
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8">
+        <v>161</v>
+      </c>
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="1">
+        <v>41395</v>
+      </c>
+      <c r="G9" s="1">
+        <v>41275</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9">
+        <v>12.0123</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1">
+        <v>40909</v>
+      </c>
+      <c r="G10" s="1">
+        <v>41030</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10">
+        <v>12.014099999999999</v>
+      </c>
+      <c r="J10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10">
+        <v>161</v>
+      </c>
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1">
+        <v>41395</v>
+      </c>
+      <c r="G11" s="1">
+        <v>41275</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11">
+        <v>12.0123</v>
+      </c>
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>18</v>
       </c>
-      <c r="M3" t="s">
-        <v>16</v>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="1">
+        <v>40909</v>
+      </c>
+      <c r="G12" s="1">
+        <v>41030</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12">
+        <v>12.0143</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12">
+        <v>161</v>
+      </c>
+      <c r="M12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1">
+        <v>41395</v>
+      </c>
+      <c r="G13" s="1">
+        <v>41275</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13">
+        <v>12.0123</v>
+      </c>
+      <c r="J13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="1">
+        <v>40909</v>
+      </c>
+      <c r="G14" s="1">
+        <v>41030</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14">
+        <v>13.0143</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14">
+        <v>161</v>
+      </c>
+      <c r="M14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>